<commit_message>
added basic reading and printing for the schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://traditionalclubs-my.sharepoint.com/personal/mkowalski_stonewallgolfclub_com/Documents/Schedules/2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lnaty\PycharmProjects\ScheduleReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{761B3AAE-17BD-4C35-BD1C-24646A6BA930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A76319AE-590E-413A-BE49-B87B6005F2D9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE255F9-81F9-4242-B019-5080B8395736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8BAC5CC-393C-44D7-A7AB-0D88649C8E3A}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="10134" xr2:uid="{A8BAC5CC-393C-44D7-A7AB-0D88649C8E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="152">
   <si>
     <t>GOLF SHOP</t>
   </si>
@@ -170,9 +170,6 @@
     <t>703-994-6571</t>
   </si>
   <si>
-    <t>10 - 3 (M)</t>
-  </si>
-  <si>
     <t>Art Garrison</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>703-401-5783</t>
   </si>
   <si>
-    <t>9 - 2 (M)</t>
-  </si>
-  <si>
     <t>Aaron Marsh</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>703-509-7635</t>
   </si>
   <si>
-    <t>6 - 1 (S)</t>
-  </si>
-  <si>
     <t>9 - 3</t>
   </si>
   <si>
@@ -485,66 +476,6 @@
     <t>703-328-0998</t>
   </si>
   <si>
-    <t>Requested Time Off</t>
-  </si>
-  <si>
-    <t>9:30 AM SG</t>
-  </si>
-  <si>
-    <t>Ladies League</t>
-  </si>
-  <si>
-    <t>Mens League</t>
-  </si>
-  <si>
-    <t>Friday Night</t>
-  </si>
-  <si>
-    <t>9:00 AM SG</t>
-  </si>
-  <si>
-    <t>Hit The Green</t>
-  </si>
-  <si>
-    <t>68 ppl</t>
-  </si>
-  <si>
-    <t>9:00AM SG</t>
-  </si>
-  <si>
-    <t>League 3:30 TT</t>
-  </si>
-  <si>
-    <t>8:30 AM SG</t>
-  </si>
-  <si>
-    <t>144 ppl</t>
-  </si>
-  <si>
-    <t>120 ppl</t>
-  </si>
-  <si>
-    <t>Back To School</t>
-  </si>
-  <si>
-    <t>Tuesday Night</t>
-  </si>
-  <si>
-    <t>Spark Golf</t>
-  </si>
-  <si>
-    <t>Call Before Coming In</t>
-  </si>
-  <si>
-    <t>League 4:30 TT</t>
-  </si>
-  <si>
-    <t>5:30 SG</t>
-  </si>
-  <si>
-    <t>Clean Pick</t>
-  </si>
-  <si>
     <t>Riley Stever</t>
   </si>
   <si>
@@ -555,22 +486,20 @@
   </si>
   <si>
     <t>Meghan Adams</t>
+  </si>
+  <si>
+    <t>10 - 3</t>
+  </si>
+  <si>
+    <t>9 - 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -622,7 +551,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,26 +612,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -736,171 +647,125 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,10 +781,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,33 +1103,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R66"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.26171875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.15625" customWidth="1"/>
+    <col min="2" max="3" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.68359375" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.41796875" customWidth="1"/>
+    <col min="11" max="11" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.41796875" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.15625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2">
@@ -1316,7 +1177,7 @@
       </c>
       <c r="R1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1366,12 +1227,12 @@
       </c>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10"/>
@@ -1394,7 +1255,7 @@
       </c>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -1436,7 +1297,7 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
@@ -1474,7 +1335,7 @@
       <c r="Q5" s="21"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
@@ -1516,7 +1377,7 @@
       <c r="Q6" s="22"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -1550,7 +1411,7 @@
       </c>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -1582,7 +1443,7 @@
       <c r="Q8" s="20"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -1618,9 +1479,9 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" s="8" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>36</v>
@@ -1648,7 +1509,7 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
@@ -1678,7 +1539,7 @@
       </c>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A12" s="8" t="s">
         <v>39</v>
       </c>
@@ -1704,7 +1565,7 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A13" s="25" t="s">
         <v>41</v>
       </c>
@@ -1726,7 +1587,7 @@
       <c r="Q13" s="27"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A14" s="28" t="s">
         <v>42</v>
       </c>
@@ -1737,7 +1598,7 @@
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="29"/>
@@ -1747,19 +1608,19 @@
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="31"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="18"/>
@@ -1776,18 +1637,18 @@
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
       <c r="O15" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>49</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>31</v>
@@ -1804,7 +1665,7 @@
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -1812,12 +1673,12 @@
       <c r="Q16" s="18"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A17" s="32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="18"/>
@@ -1834,18 +1695,18 @@
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
       <c r="O17" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="5"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A18" s="32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="18"/>
@@ -1864,12 +1725,12 @@
       <c r="Q18" s="18"/>
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="18"/>
@@ -1888,12 +1749,12 @@
       <c r="Q19" s="18"/>
       <c r="R19" s="5"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="18"/>
@@ -1916,12 +1777,12 @@
       <c r="Q20" s="18"/>
       <c r="R20" s="5"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="18" t="s">
@@ -1944,12 +1805,12 @@
       <c r="Q21" s="18"/>
       <c r="R21" s="5"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="18"/>
@@ -1958,7 +1819,7 @@
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
       <c r="I22" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="9"/>
@@ -1968,23 +1829,23 @@
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
@@ -1994,23 +1855,23 @@
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="P23" s="18"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="5"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -2025,12 +1886,12 @@
       <c r="Q24" s="18"/>
       <c r="R24" s="5"/>
     </row>
-    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A25" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="18"/>
@@ -2038,7 +1899,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="3"/>
@@ -2048,17 +1909,17 @@
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
       <c r="P25" s="18" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="Q25" s="18"/>
       <c r="R25" s="5"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="18"/>
@@ -2074,14 +1935,14 @@
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
       <c r="P26" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q26" s="18"/>
       <c r="R26" s="5"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="34"/>
@@ -2101,18 +1962,18 @@
       <c r="Q27" s="34"/>
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="11" t="s">
@@ -2123,7 +1984,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
@@ -2133,12 +1994,12 @@
       </c>
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>21</v>
@@ -2162,7 +2023,7 @@
       </c>
       <c r="M29" s="18"/>
       <c r="N29" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O29" s="18" t="s">
         <v>35</v>
@@ -2171,12 +2032,12 @@
       <c r="Q29" s="21"/>
       <c r="R29" s="5"/>
     </row>
-    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A30" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
@@ -2188,7 +2049,7 @@
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I30" s="21"/>
       <c r="J30" s="3"/>
@@ -2198,7 +2059,7 @@
       <c r="L30" s="9"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O30" s="18" t="s">
         <v>35</v>
@@ -2209,19 +2070,19 @@
       <c r="Q30" s="9"/>
       <c r="R30" s="5"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="33"/>
       <c r="G31" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
@@ -2231,7 +2092,7 @@
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
       <c r="O31" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P31" s="18" t="s">
         <v>15</v>
@@ -2239,22 +2100,22 @@
       <c r="Q31" s="18"/>
       <c r="R31" s="31"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="20"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>15</v>
@@ -2262,27 +2123,27 @@
       <c r="J32" s="30"/>
       <c r="K32" s="9"/>
       <c r="L32" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M32" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N32" s="18"/>
       <c r="O32" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P32" s="18"/>
       <c r="Q32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R32" s="31"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="R32" s="31"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>16</v>
@@ -2294,14 +2155,14 @@
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
       <c r="H33" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="30"/>
       <c r="K33" s="9"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N33" s="20"/>
       <c r="O33" s="20"/>
@@ -2309,17 +2170,17 @@
       <c r="Q33" s="20"/>
       <c r="R33" s="31"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>19</v>
@@ -2330,14 +2191,14 @@
       <c r="J34" s="30"/>
       <c r="K34" s="21"/>
       <c r="L34" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M34" s="18"/>
       <c r="N34" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O34" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P34" s="18"/>
       <c r="Q34" s="18" t="s">
@@ -2345,12 +2206,12 @@
       </c>
       <c r="R34" s="31"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="20"/>
@@ -2368,21 +2229,21 @@
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
       <c r="N35" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O35" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="31"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="18"/>
@@ -2405,12 +2266,12 @@
       </c>
       <c r="R36" s="31"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="9"/>
@@ -2428,17 +2289,17 @@
       <c r="N37" s="18"/>
       <c r="O37" s="9"/>
       <c r="P37" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q37" s="18"/>
       <c r="R37" s="31"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>19</v>
@@ -2447,19 +2308,19 @@
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
       <c r="G38" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H38" s="18"/>
       <c r="I38" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J38" s="30"/>
       <c r="K38" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L38" s="9"/>
       <c r="M38" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N38" s="18"/>
       <c r="O38" s="21"/>
@@ -2467,12 +2328,12 @@
       <c r="Q38" s="21"/>
       <c r="R38" s="31"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="9"/>
@@ -2480,7 +2341,7 @@
       <c r="F39" s="18"/>
       <c r="G39" s="9"/>
       <c r="H39" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="30"/>
@@ -2490,17 +2351,17 @@
       <c r="N39" s="18"/>
       <c r="O39" s="9"/>
       <c r="P39" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q39" s="9"/>
       <c r="R39" s="31"/>
     </row>
-    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A40" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="9"/>
@@ -2508,7 +2369,7 @@
       <c r="F40" s="18"/>
       <c r="G40" s="33"/>
       <c r="H40" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I40" s="18"/>
       <c r="J40" s="3"/>
@@ -2518,23 +2379,23 @@
       <c r="N40" s="18"/>
       <c r="O40" s="33"/>
       <c r="P40" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q40" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R40" s="5"/>
     </row>
-    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A41" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>21</v>
@@ -2543,48 +2404,48 @@
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9" t="s">
         <v>21</v>
       </c>
       <c r="N41" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O41" s="18"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
       <c r="R41" s="5"/>
     </row>
-    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A42" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E42" s="18"/>
       <c r="F42" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H42" s="21"/>
       <c r="I42" s="9"/>
       <c r="J42" s="3"/>
       <c r="K42" s="9"/>
       <c r="L42" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M42" s="18" t="s">
         <v>19</v>
@@ -2592,17 +2453,17 @@
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
       <c r="P42" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q42" s="9"/>
       <c r="R42" s="5"/>
     </row>
-    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A43" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>19</v>
@@ -2624,21 +2485,21 @@
       <c r="L43" s="9"/>
       <c r="M43" s="18"/>
       <c r="N43" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O43" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P43" s="9"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="5"/>
     </row>
-    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A44" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21"/>
@@ -2657,12 +2518,12 @@
       <c r="Q44" s="18"/>
       <c r="R44" s="5"/>
     </row>
-    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A45" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>19</v>
@@ -2672,88 +2533,88 @@
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="9"/>
       <c r="I45" s="18" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="18"/>
       <c r="N45" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O45" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R45" s="5"/>
     </row>
-    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A46" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F46" s="18"/>
       <c r="G46" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="18"/>
       <c r="J46" s="3"/>
       <c r="K46" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="18"/>
       <c r="N46" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O46" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P46" s="21"/>
       <c r="Q46" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="R46" s="5"/>
     </row>
-    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A47" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E47" s="18"/>
       <c r="F47" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="9"/>
       <c r="I47" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="9"/>
@@ -2762,7 +2623,7 @@
       </c>
       <c r="M47" s="18"/>
       <c r="N47" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O47" s="18"/>
       <c r="P47" s="9" t="s">
@@ -2771,12 +2632,12 @@
       <c r="Q47" s="18"/>
       <c r="R47" s="5"/>
     </row>
-    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A48" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -2794,19 +2655,19 @@
         <v>15</v>
       </c>
       <c r="N48" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O48" s="18"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="18"/>
       <c r="R48" s="5"/>
     </row>
-    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A49" s="8" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
@@ -2815,7 +2676,7 @@
       <c r="G49" s="20"/>
       <c r="H49" s="18"/>
       <c r="I49" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="21"/>
@@ -2827,19 +2688,19 @@
       <c r="Q49" s="21"/>
       <c r="R49" s="5"/>
     </row>
-    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A50" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
@@ -2847,32 +2708,32 @@
       <c r="I50" s="18"/>
       <c r="J50" s="3"/>
       <c r="K50" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L50" s="9"/>
       <c r="M50" s="18" t="s">
         <v>21</v>
       </c>
       <c r="N50" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="O50" s="18"/>
       <c r="P50" s="9"/>
       <c r="Q50" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R50" s="5"/>
     </row>
-    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A51" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C51" s="20"/>
       <c r="D51" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="18"/>
@@ -2882,7 +2743,7 @@
       <c r="J51" s="3"/>
       <c r="K51" s="20"/>
       <c r="L51" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M51" s="20"/>
       <c r="N51" s="18"/>
@@ -2891,12 +2752,12 @@
       <c r="Q51" s="20"/>
       <c r="R51" s="5"/>
     </row>
-    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A52" s="36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="18"/>
@@ -2909,7 +2770,7 @@
       </c>
       <c r="H52" s="33"/>
       <c r="I52" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J52" s="38"/>
       <c r="K52" s="33"/>
@@ -2918,18 +2779,18 @@
       </c>
       <c r="M52" s="33"/>
       <c r="N52" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O52" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="P52" s="33"/>
       <c r="Q52" s="33"/>
       <c r="R52" s="5"/>
     </row>
-    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A53" s="25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="39"/>
@@ -2949,24 +2810,24 @@
       <c r="Q53" s="39"/>
       <c r="R53" s="5"/>
     </row>
-    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A54" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F54" s="33"/>
       <c r="G54" s="11"/>
       <c r="H54" s="42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I54" s="9"/>
       <c r="J54" s="3"/>
@@ -2974,26 +2835,26 @@
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54" s="11" t="s">
         <v>19</v>
       </c>
       <c r="Q54" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="R54" s="5"/>
+    </row>
+    <row r="55" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="R54" s="5"/>
-    </row>
-    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
@@ -3001,7 +2862,7 @@
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="11"/>
@@ -3010,31 +2871,31 @@
       <c r="N55" s="22"/>
       <c r="O55" s="11"/>
       <c r="P55" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Q55" s="42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R55" s="5"/>
     </row>
-    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A56" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I56" s="9"/>
       <c r="J56" s="3"/>
@@ -3047,22 +2908,22 @@
       <c r="Q56" s="21"/>
       <c r="R56" s="5"/>
     </row>
-    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A57" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G57" s="11"/>
       <c r="H57" s="42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I57" s="9"/>
       <c r="J57" s="3"/>
@@ -3077,19 +2938,19 @@
       <c r="Q57" s="21"/>
       <c r="R57" s="5"/>
     </row>
-    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A58" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="33"/>
       <c r="G58" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H58" s="11"/>
       <c r="I58" s="9"/>
@@ -3098,63 +2959,63 @@
       <c r="L58" s="10"/>
       <c r="M58" s="44"/>
       <c r="N58" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O58" s="16"/>
       <c r="P58" s="16"/>
       <c r="Q58" s="21"/>
       <c r="R58" s="5"/>
     </row>
-    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A59" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="16"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L59" s="11"/>
       <c r="M59" s="18"/>
       <c r="N59" s="16"/>
       <c r="O59" s="18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P59" s="11"/>
       <c r="Q59" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R59" s="5"/>
     </row>
-    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A60" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="18"/>
       <c r="E60" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I60" s="9"/>
       <c r="J60" s="5"/>
@@ -3163,15 +3024,15 @@
       <c r="M60" s="18"/>
       <c r="N60" s="11"/>
       <c r="O60" s="18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="P60" s="11"/>
       <c r="Q60" s="45" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="R60" s="5"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="46"/>
       <c r="B61" s="46"/>
       <c r="C61" s="47"/>
@@ -3191,103 +3052,6 @@
       <c r="Q61" s="47"/>
       <c r="R61" s="47"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="C62" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="E62" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="G62" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="L62" s="49" t="s">
-        <v>151</v>
-      </c>
-      <c r="M62" s="51" t="s">
-        <v>152</v>
-      </c>
-      <c r="N62" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="O62" s="49" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="C63" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D63" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="E63" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="G63" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="L63" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="M63" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="N63" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="O63" s="53" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="D64" s="51" t="s">
-        <v>163</v>
-      </c>
-      <c r="E64" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="L64" s="51" t="s">
-        <v>163</v>
-      </c>
-      <c r="M64" s="49" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="56" t="s">
-        <v>165</v>
-      </c>
-      <c r="D65" s="54" t="s">
-        <v>166</v>
-      </c>
-      <c r="E65" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="L65" s="54" t="s">
-        <v>166</v>
-      </c>
-      <c r="M65" s="53" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E66" s="57" t="s">
-        <v>168</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" fitToWidth="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>